<commit_message>
add enhence equip local
</commit_message>
<xml_diff>
--- a/localization_cn.xlsx
+++ b/localization_cn.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="318">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1215,6 +1215,62 @@
   </si>
   <si>
     <t>需要更多的[img:mainscene/MM_makalong.png]。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_START</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始强化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_COST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_CONSUME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗装备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_TITLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备强化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_TARGET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择强化装备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXT_ENHENCE_CHOOSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择消耗装备</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1569,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2875,6 +2931,62 @@
       </c>
       <c r="B162" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A163" t="s">
+        <v>304</v>
+      </c>
+      <c r="B163" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A164" t="s">
+        <v>306</v>
+      </c>
+      <c r="B164" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A165" t="s">
+        <v>308</v>
+      </c>
+      <c r="B165" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A166" t="s">
+        <v>310</v>
+      </c>
+      <c r="B166" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A167" t="s">
+        <v>312</v>
+      </c>
+      <c r="B167" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A168" t="s">
+        <v>314</v>
+      </c>
+      <c r="B168" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A169" t="s">
+        <v>316</v>
+      </c>
+      <c r="B169" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>